<commit_message>
Atualiza calculos acerto conta campinho
</commit_message>
<xml_diff>
--- a/praça dos lavradores/VENDA/CALCULOS.xlsx
+++ b/praça dos lavradores/VENDA/CALCULOS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.bfn\Desktop\imoveis\praça dos lavradores\VENDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F466DFD9-2DBB-4F34-84B8-C57777242FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B7F0B0-ED34-4C07-A983-91CDC3863582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{69638CC1-6141-47C6-B7A1-94B499BBE744}"/>
+    <workbookView xWindow="-38520" yWindow="-3525" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{69638CC1-6141-47C6-B7A1-94B499BBE744}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>SINAL</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>SALDO DEVEDOR NÃO QUITADO COM RECURSOS PRÓPRIOS</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>IPTU 2023 (R$ 926,00) proporcional</t>
+  </si>
+  <si>
+    <t>Condomínio (25/08 até  31/08) (R$610,54) proporcional</t>
   </si>
 </sst>
 </file>
@@ -103,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +122,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -145,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -160,6 +175,10 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -560,7 +579,7 @@
         <v>1734</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ref="I7:I11" si="1">I8-G9</f>
+        <f t="shared" ref="I9:I11" si="1">I8-G9</f>
         <v>173400</v>
       </c>
     </row>
@@ -584,16 +603,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2978DD79-AEF9-414F-B090-CC87296ED2A8}">
-  <dimension ref="D6:F10"/>
+  <dimension ref="D6:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="32.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -640,6 +659,33 @@
         <v>4760</v>
       </c>
     </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="4">
+        <f>926/12*4</f>
+        <v>308.66666666666669</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="4">
+        <f>610.54/30*6</f>
+        <v>122.108</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9">
+        <f>SUM(E14:E15)</f>
+        <v>430.77466666666669</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>